<commit_message>
update the Registration page Test Case
</commit_message>
<xml_diff>
--- a/OpenCart-Test Scenarios .xlsx
+++ b/OpenCart-Test Scenarios .xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\SQA Projects\OpenCart (eCommerce)\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886B768E-904F-49BE-917F-A57B3529D9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1800" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="1" r:id="rId1"/>
@@ -273,7 +279,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -423,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -476,17 +482,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -761,18 +770,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B7" sqref="A2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -789,58 +798,58 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="19"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="19"/>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="19"/>
+      <c r="B4" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="20"/>
     </row>
     <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="19"/>
-    </row>
-    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="C5" s="20"/>
+    </row>
+    <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="21">
         <v>44533</v>
       </c>
-      <c r="C6" s="19"/>
-    </row>
-    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="21">
         <v>44537</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="22"/>
     </row>
     <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">

</xml_diff>